<commit_message>
En proceso de crear el valuador asíncrono. Se me acabaron las requests disponibles diarias de Pricely.
</commit_message>
<xml_diff>
--- a/assets/tabla-intermedia.xlsx
+++ b/assets/tabla-intermedia.xlsx
@@ -1,14 +1,23 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:mv="urn:schemas-microsoft-com:mac:vml" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24332"/>
   <workbookPr/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\nicob\OneDrive\Escritorio\ilporco-comparador\assets\"/>
+    </mc:Choice>
+  </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2FDE73A3-251C-4B60-B91F-CD18DD1B33A8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <bookViews>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+  </bookViews>
   <sheets>
-    <sheet state="visible" name="Hoja1" sheetId="1" r:id="rId4"/>
-    <sheet state="visible" name="Hoja2" sheetId="2" r:id="rId5"/>
-    <sheet state="visible" name="Hoja3" sheetId="3" r:id="rId6"/>
+    <sheet name="Hoja1" sheetId="1" r:id="rId1"/>
+    <sheet name="Hoja2" sheetId="2" r:id="rId2"/>
+    <sheet name="Hoja3" sheetId="3" r:id="rId3"/>
   </sheets>
-  <definedNames/>
-  <calcPr/>
+  <calcPr calcId="0"/>
   <extLst>
     <ext uri="GoogleSheetsCustomDataVersion2">
       <go:sheetsCustomData xmlns:go="http://customooxmlschemas.google.com/" r:id="rId7" roundtripDataChecksum="8tDhiZ+uUNjSkePvAESug0gdiWsEzhErKiIEoI26VPk="/>
@@ -18,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="99" uniqueCount="99">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="92" uniqueCount="92">
   <si>
     <t>Artículos</t>
   </si>
@@ -67,15 +76,17 @@
   <si>
     <r>
       <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
         <rFont val="Calibri"/>
-        <color theme="1"/>
       </rPr>
       <t xml:space="preserve">491 </t>
     </r>
     <r>
       <rPr>
+        <sz val="11"/>
+        <color rgb="FFFF0000"/>
         <rFont val="Calibri"/>
-        <color rgb="FFFF0000"/>
       </rPr>
       <t>!</t>
     </r>
@@ -102,24 +113,6 @@
     <t>SOPRESATA PIEZA EV</t>
   </si>
   <si>
-    <r>
-      <rPr>
-        <rFont val="__inter_855b4d, __inter_Fallback_855b4d"/>
-        <color rgb="FFA1A1AA"/>
-        <sz val="9.0"/>
-      </rPr>
-      <t xml:space="preserve">7798013100246 </t>
-    </r>
-    <r>
-      <rPr>
-        <rFont val="__inter_855b4d, __inter_Fallback_855b4d"/>
-        <color rgb="FFFF0000"/>
-        <sz val="9.0"/>
-      </rPr>
-      <t>!</t>
-    </r>
-  </si>
-  <si>
     <t>SALAME COLONIA PIEZA EV</t>
   </si>
   <si>
@@ -168,63 +161,9 @@
     <t xml:space="preserve"> </t>
   </si>
   <si>
-    <r>
-      <rPr>
-        <rFont val="__inter_855b4d, __inter_Fallback_855b4d"/>
-        <color rgb="FFA1A1AA"/>
-        <sz val="9.0"/>
-      </rPr>
-      <t xml:space="preserve"> 2009380000004 </t>
-    </r>
-    <r>
-      <rPr>
-        <rFont val="__inter_855b4d, __inter_Fallback_855b4d"/>
-        <color rgb="FFFF0000"/>
-        <sz val="9.0"/>
-      </rPr>
-      <t>!</t>
-    </r>
-  </si>
-  <si>
     <t>LEBERWURST PIEZA EV</t>
   </si>
   <si>
-    <r>
-      <rPr>
-        <rFont val="__inter_855b4d, __inter_Fallback_855b4d"/>
-        <color rgb="FFA1A1AA"/>
-        <sz val="9.0"/>
-      </rPr>
-      <t xml:space="preserve">7798013107726 </t>
-    </r>
-    <r>
-      <rPr>
-        <rFont val="__inter_855b4d, __inter_Fallback_855b4d"/>
-        <color rgb="FFFF0000"/>
-        <sz val="9.0"/>
-      </rPr>
-      <t>!</t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <rPr>
-        <rFont val="__inter_855b4d, __inter_Fallback_855b4d"/>
-        <color rgb="FFA1A1AA"/>
-        <sz val="9.0"/>
-      </rPr>
-      <t xml:space="preserve">7798183684102 </t>
-    </r>
-    <r>
-      <rPr>
-        <rFont val="__inter_855b4d, __inter_Fallback_855b4d"/>
-        <color rgb="FFFF0000"/>
-        <sz val="9.0"/>
-      </rPr>
-      <t>!</t>
-    </r>
-  </si>
-  <si>
     <t>QUESO DE CERDO PIEZA EV</t>
   </si>
   <si>
@@ -276,24 +215,6 @@
     <t>MORTADELA TRADICIONAL PIEZA EV</t>
   </si>
   <si>
-    <r>
-      <rPr>
-        <rFont val="__inter_855b4d, __inter_Fallback_855b4d"/>
-        <color rgb="FFA1A1AA"/>
-        <sz val="9.0"/>
-      </rPr>
-      <t xml:space="preserve">7798183683556 </t>
-    </r>
-    <r>
-      <rPr>
-        <rFont val="__inter_855b4d, __inter_Fallback_855b4d"/>
-        <color rgb="FFFF0000"/>
-        <sz val="9.0"/>
-      </rPr>
-      <t>!</t>
-    </r>
-  </si>
-  <si>
     <t>JAMON HORNEADO AHUMADO FETEADO EV</t>
   </si>
   <si>
@@ -306,24 +227,6 @@
     <t>MORTADELA C/ QUESO PIEZA EV</t>
   </si>
   <si>
-    <r>
-      <rPr>
-        <rFont val="__inter_855b4d, __inter_Fallback_855b4d"/>
-        <color rgb="FFA1A1AA"/>
-        <sz val="9.0"/>
-      </rPr>
-      <t xml:space="preserve">7790079019913 </t>
-    </r>
-    <r>
-      <rPr>
-        <rFont val="__inter_855b4d, __inter_Fallback_855b4d"/>
-        <color rgb="FFFF0000"/>
-        <sz val="9.0"/>
-      </rPr>
-      <t>!</t>
-    </r>
-  </si>
-  <si>
     <t>SALCHICHAS VIENA CON QUESO EV</t>
   </si>
   <si>
@@ -379,24 +282,6 @@
   </si>
   <si>
     <t>JAMON CRUDO FETEADO EV</t>
-  </si>
-  <si>
-    <r>
-      <rPr>
-        <rFont val="__inter_855b4d, __inter_Fallback_855b4d"/>
-        <color rgb="FFA1A1AA"/>
-        <sz val="9.0"/>
-      </rPr>
-      <t xml:space="preserve">7798016105668 </t>
-    </r>
-    <r>
-      <rPr>
-        <rFont val="__inter_855b4d, __inter_Fallback_855b4d"/>
-        <color rgb="FFFF0000"/>
-        <sz val="9.0"/>
-      </rPr>
-      <t>!</t>
-    </r>
   </si>
   <si>
     <t>PANCETA SALADA PIEZA EV</t>
@@ -438,41 +323,47 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <fonts count="7">
     <font>
-      <sz val="11.0"/>
+      <sz val="11"/>
       <color theme="1"/>
       <name val="Calibri"/>
       <scheme val="minor"/>
     </font>
     <font>
       <b/>
-      <sz val="11.0"/>
+      <sz val="11"/>
       <color theme="1"/>
       <name val="Calibri"/>
     </font>
-    <font/>
     <font>
       <b/>
+      <sz val="11"/>
       <color theme="1"/>
       <name val="Calibri"/>
       <scheme val="minor"/>
     </font>
     <font>
-      <sz val="11.0"/>
+      <sz val="11"/>
       <color theme="1"/>
       <name val="Calibri"/>
     </font>
     <font>
-      <sz val="9.0"/>
+      <sz val="9"/>
       <color rgb="FFA1A1AA"/>
       <name val="__inter_855b4d"/>
     </font>
     <font>
+      <sz val="11"/>
       <color theme="1"/>
       <name val="Calibri"/>
       <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FFFF0000"/>
+      <name val="Calibri"/>
     </font>
   </fonts>
   <fills count="6">
@@ -480,7 +371,7 @@
       <patternFill patternType="none"/>
     </fill>
     <fill>
-      <patternFill patternType="lightGray"/>
+      <patternFill patternType="gray125"/>
     </fill>
     <fill>
       <patternFill patternType="solid">
@@ -507,84 +398,68 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="4">
-    <border/>
+  <borders count="2">
     <border>
       <left/>
-      <top/>
-      <bottom/>
-    </border>
-    <border>
-      <top/>
-      <bottom/>
-    </border>
-    <border>
       <right/>
       <top/>
       <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom/>
+      <diagonal/>
     </border>
   </borders>
   <cellStyleXfs count="1">
-    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" applyAlignment="1" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="13">
-    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
-      <alignment readingOrder="0" shrinkToFit="0" vertical="bottom" wrapText="0"/>
+  <cellXfs count="11">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="2" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
     </xf>
-    <xf borderId="1" fillId="2" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFill="1" applyFont="1">
-      <alignment horizontal="center" readingOrder="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
     </xf>
-    <xf borderId="2" fillId="0" fontId="2" numFmtId="0" xfId="0" applyBorder="1" applyFont="1"/>
-    <xf borderId="3" fillId="0" fontId="2" numFmtId="0" xfId="0" applyBorder="1" applyFont="1"/>
-    <xf borderId="0" fillId="3" fontId="3" numFmtId="0" xfId="0" applyAlignment="1" applyFill="1" applyFont="1">
-      <alignment horizontal="center" readingOrder="0" textRotation="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf borderId="0" fillId="4" fontId="3" numFmtId="0" xfId="0" applyAlignment="1" applyFill="1" applyFont="1">
-      <alignment horizontal="center" readingOrder="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
     </xf>
-    <xf borderId="0" fillId="0" fontId="3" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
-      <alignment horizontal="center" readingOrder="0"/>
+    <xf numFmtId="49" fontId="4" fillId="5" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="4" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
     </xf>
-    <xf borderId="0" fillId="0" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
-      <alignment horizontal="center" shrinkToFit="0" vertical="center" wrapText="1"/>
-    </xf>
-    <xf borderId="0" fillId="0" fontId="3" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
-      <alignment readingOrder="0"/>
-    </xf>
-    <xf borderId="0" fillId="0" fontId="4" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
-      <alignment shrinkToFit="0" vertical="center" wrapText="1"/>
-    </xf>
-    <xf borderId="0" fillId="5" fontId="5" numFmtId="49" xfId="0" applyAlignment="1" applyFill="1" applyFont="1" applyNumberFormat="1">
-      <alignment readingOrder="0"/>
-    </xf>
-    <xf borderId="0" fillId="0" fontId="6" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
-      <alignment readingOrder="0"/>
-    </xf>
-    <xf borderId="0" fillId="5" fontId="5" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
-      <alignment readingOrder="0"/>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
-    <cellStyle xfId="0" name="Normal" builtinId="0"/>
+    <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
+  <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
+      <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
+    </ext>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
+      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
+    </ext>
+  </extLst>
 </styleSheet>
 </file>
 
-<file path=xl/drawings/drawing1.xml><?xml version="1.0" encoding="utf-8"?>
-<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:cx="http://schemas.microsoft.com/office/drawing/2014/chartex" xmlns:cx1="http://schemas.microsoft.com/office/drawing/2015/9/8/chartex" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:dgm="http://schemas.openxmlformats.org/drawingml/2006/diagram" xmlns:x3Unk="http://schemas.microsoft.com/office/drawing/2010/slicer" xmlns:sle15="http://schemas.microsoft.com/office/drawing/2012/slicer"/>
-</file>
-
-<file path=xl/drawings/drawing2.xml><?xml version="1.0" encoding="utf-8"?>
-<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:cx="http://schemas.microsoft.com/office/drawing/2014/chartex" xmlns:cx1="http://schemas.microsoft.com/office/drawing/2015/9/8/chartex" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:dgm="http://schemas.openxmlformats.org/drawingml/2006/diagram" xmlns:x3Unk="http://schemas.microsoft.com/office/drawing/2010/slicer" xmlns:sle15="http://schemas.microsoft.com/office/drawing/2012/slicer"/>
-</file>
-
-<file path=xl/drawings/drawing3.xml><?xml version="1.0" encoding="utf-8"?>
-<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:cx="http://schemas.microsoft.com/office/drawing/2014/chartex" xmlns:cx1="http://schemas.microsoft.com/office/drawing/2015/9/8/chartex" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:dgm="http://schemas.openxmlformats.org/drawingml/2006/diagram" xmlns:x3Unk="http://schemas.microsoft.com/office/drawing/2010/slicer" xmlns:sle15="http://schemas.microsoft.com/office/drawing/2012/slicer"/>
-</file>
-
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="Sheets">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Sheets">
   <a:themeElements>
     <a:clrScheme name="Sheets">
       <a:dk1>
@@ -774,1094 +649,1101 @@
       </a:bgFillStyleLst>
     </a:fmtScheme>
   </a:themeElements>
+  <a:objectDefaults/>
+  <a:extraClrSchemeLst/>
 </a:theme>
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:mv="urn:schemas-microsoft-com:mac:vml" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
-  <sheetPr>
-    <pageSetUpPr/>
-  </sheetPr>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+  <dimension ref="A1:P1000"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="I67" sqref="I67"/>
+    </sheetView>
   </sheetViews>
-  <sheetFormatPr customHeight="1" defaultColWidth="14.43" defaultRowHeight="15.0"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="14.42578125" defaultRowHeight="15" customHeight="1"/>
   <cols>
-    <col customWidth="1" min="1" max="2" width="20.71"/>
-    <col customWidth="1" min="3" max="3" width="58.29"/>
-    <col customWidth="1" min="4" max="4" width="15.29"/>
-    <col customWidth="1" min="5" max="7" width="10.71"/>
-    <col customWidth="1" min="8" max="8" width="22.86"/>
-    <col customWidth="1" min="9" max="9" width="19.57"/>
-    <col customWidth="1" min="10" max="10" width="25.43"/>
-    <col customWidth="1" min="11" max="15" width="10.71"/>
-    <col customWidth="1" min="16" max="16" width="13.57"/>
-    <col customWidth="1" min="17" max="22" width="10.71"/>
+    <col min="1" max="2" width="20.7109375" customWidth="1"/>
+    <col min="3" max="3" width="58.28515625" customWidth="1"/>
+    <col min="4" max="4" width="15.28515625" customWidth="1"/>
+    <col min="5" max="7" width="10.7109375" customWidth="1"/>
+    <col min="8" max="8" width="22.85546875" customWidth="1"/>
+    <col min="9" max="9" width="19.5703125" customWidth="1"/>
+    <col min="10" max="10" width="25.42578125" customWidth="1"/>
+    <col min="11" max="15" width="10.7109375" customWidth="1"/>
+    <col min="16" max="16" width="13.5703125" customWidth="1"/>
+    <col min="17" max="22" width="10.7109375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1">
-      <c r="A1" s="1" t="s">
+    <row r="1" spans="1:16">
+      <c r="A1" s="9" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="2"/>
-      <c r="C1" s="3"/>
-      <c r="D1" s="4" t="s">
+      <c r="B1" s="9"/>
+      <c r="C1" s="9"/>
+      <c r="D1" s="10" t="s">
         <v>1</v>
       </c>
-      <c r="J1" s="5" t="s">
+      <c r="E1" s="10"/>
+      <c r="F1" s="10"/>
+      <c r="G1" s="10"/>
+      <c r="H1" s="10"/>
+      <c r="I1" s="10"/>
+      <c r="J1" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="K1" s="6"/>
-      <c r="L1" s="6"/>
-      <c r="M1" s="6"/>
-      <c r="N1" s="6"/>
-      <c r="O1" s="6"/>
-      <c r="P1" s="6"/>
-    </row>
-    <row r="2">
-      <c r="A2" s="7" t="s">
+      <c r="K1" s="2"/>
+      <c r="L1" s="2"/>
+      <c r="M1" s="2"/>
+      <c r="N1" s="2"/>
+      <c r="O1" s="2"/>
+      <c r="P1" s="2"/>
+    </row>
+    <row r="2" spans="1:16">
+      <c r="A2" s="3" t="s">
         <v>3</v>
       </c>
-      <c r="B2" s="7" t="s">
+      <c r="B2" s="3" t="s">
         <v>4</v>
       </c>
-      <c r="C2" s="7" t="s">
+      <c r="C2" s="3" t="s">
         <v>5</v>
       </c>
-      <c r="D2" s="8" t="s">
+      <c r="D2" s="4" t="s">
         <v>6</v>
       </c>
-      <c r="E2" s="8" t="s">
+      <c r="E2" s="4" t="s">
         <v>7</v>
       </c>
-      <c r="F2" s="8" t="s">
+      <c r="F2" s="4" t="s">
         <v>8</v>
       </c>
-      <c r="G2" s="8" t="s">
+      <c r="G2" s="4" t="s">
         <v>9</v>
       </c>
-      <c r="H2" s="8" t="s">
+      <c r="H2" s="4" t="s">
         <v>10</v>
       </c>
-      <c r="I2" s="8" t="s">
+      <c r="I2" s="4" t="s">
         <v>11</v>
       </c>
-      <c r="J2" s="8" t="s">
+      <c r="J2" s="4" t="s">
         <v>12</v>
       </c>
     </row>
-    <row r="3">
-      <c r="A3" s="9">
-        <v>52.0</v>
-      </c>
-      <c r="B3" s="9">
-        <v>102.0</v>
-      </c>
-      <c r="C3" s="9" t="s">
+    <row r="3" spans="1:16">
+      <c r="A3" s="5">
+        <v>52</v>
+      </c>
+      <c r="B3" s="5">
+        <v>102</v>
+      </c>
+      <c r="C3" s="5" t="s">
         <v>13</v>
       </c>
-      <c r="I3" s="10" t="s">
+      <c r="I3" s="6" t="s">
         <v>14</v>
       </c>
-      <c r="J3" s="11" t="s">
+      <c r="J3" s="7" t="s">
         <v>15</v>
       </c>
     </row>
-    <row r="4">
-      <c r="A4" s="9">
-        <v>53.0</v>
-      </c>
-      <c r="B4" s="9">
-        <v>103.0</v>
-      </c>
-      <c r="C4" s="9" t="s">
+    <row r="4" spans="1:16">
+      <c r="A4" s="5">
+        <v>53</v>
+      </c>
+      <c r="B4" s="5">
+        <v>103</v>
+      </c>
+      <c r="C4" s="5" t="s">
         <v>16</v>
       </c>
     </row>
-    <row r="5">
-      <c r="A5" s="9">
-        <v>54.0</v>
-      </c>
-      <c r="B5" s="9">
-        <v>104.0</v>
-      </c>
-      <c r="C5" s="9" t="s">
+    <row r="5" spans="1:16">
+      <c r="A5" s="5">
+        <v>54</v>
+      </c>
+      <c r="B5" s="5">
+        <v>104</v>
+      </c>
+      <c r="C5" s="5" t="s">
         <v>17</v>
       </c>
-      <c r="I5" s="12">
-        <v>2.017139000007E12</v>
-      </c>
-    </row>
-    <row r="6">
-      <c r="A6" s="9">
-        <v>57.0</v>
-      </c>
-      <c r="B6" s="9">
-        <v>107.0</v>
-      </c>
-      <c r="C6" s="9" t="s">
+      <c r="I5" s="8">
+        <v>2017139000007</v>
+      </c>
+    </row>
+    <row r="6" spans="1:16">
+      <c r="A6" s="5">
+        <v>57</v>
+      </c>
+      <c r="B6" s="5">
+        <v>107</v>
+      </c>
+      <c r="C6" s="5" t="s">
         <v>18</v>
       </c>
-      <c r="D6" s="12">
-        <v>7.798013100246E12</v>
-      </c>
-    </row>
-    <row r="7">
-      <c r="A7" s="9">
-        <v>104.0</v>
-      </c>
-      <c r="B7" s="9">
-        <v>159.0</v>
-      </c>
-      <c r="C7" s="9" t="s">
+      <c r="D6" s="8">
+        <v>7798013100246</v>
+      </c>
+    </row>
+    <row r="7" spans="1:16">
+      <c r="A7" s="5">
+        <v>104</v>
+      </c>
+      <c r="B7" s="5">
+        <v>159</v>
+      </c>
+      <c r="C7" s="5" t="s">
         <v>19</v>
       </c>
-      <c r="D7" s="12">
-        <v>2.512038000009E12</v>
-      </c>
-      <c r="G7" s="12">
-        <v>2.000000160733E12</v>
-      </c>
-      <c r="I7" s="12">
-        <v>2.595472000002E12</v>
-      </c>
-    </row>
-    <row r="8">
-      <c r="A8" s="9">
-        <v>163.0</v>
-      </c>
-      <c r="B8" s="9">
-        <v>344.0</v>
-      </c>
-      <c r="C8" s="9" t="s">
+      <c r="D7" s="8">
+        <v>2512038000009</v>
+      </c>
+      <c r="G7" s="8">
+        <v>2000000160733</v>
+      </c>
+      <c r="I7" s="8">
+        <v>2595472000002</v>
+      </c>
+    </row>
+    <row r="8" spans="1:16">
+      <c r="A8" s="5">
+        <v>163</v>
+      </c>
+      <c r="B8" s="5">
+        <v>344</v>
+      </c>
+      <c r="C8" s="5" t="s">
         <v>20</v>
       </c>
-      <c r="D8" s="12">
-        <v>2.0036379E12</v>
-      </c>
-      <c r="I8" s="12">
-        <v>2.034910000001E12</v>
-      </c>
-      <c r="J8" s="11">
-        <v>135.0</v>
-      </c>
-    </row>
-    <row r="9">
-      <c r="A9" s="9">
-        <v>190.0</v>
-      </c>
-      <c r="B9" s="9">
-        <v>411.0</v>
-      </c>
-      <c r="C9" s="9" t="s">
+      <c r="D8" s="8">
+        <v>2003637900000</v>
+      </c>
+      <c r="I8" s="8">
+        <v>2034910000001</v>
+      </c>
+      <c r="J8" s="7">
+        <v>135</v>
+      </c>
+    </row>
+    <row r="9" spans="1:16">
+      <c r="A9" s="5">
+        <v>190</v>
+      </c>
+      <c r="B9" s="5">
+        <v>411</v>
+      </c>
+      <c r="C9" s="5" t="s">
         <v>21</v>
       </c>
-      <c r="I9" s="12">
-        <v>2.000212000001E12</v>
-      </c>
-    </row>
-    <row r="10">
-      <c r="A10" s="9">
-        <v>191.0</v>
-      </c>
-      <c r="B10" s="9">
-        <v>412.0</v>
-      </c>
-      <c r="C10" s="9" t="s">
+      <c r="I9" s="8">
+        <v>2000212000001</v>
+      </c>
+    </row>
+    <row r="10" spans="1:16">
+      <c r="A10" s="5">
+        <v>191</v>
+      </c>
+      <c r="B10" s="5">
+        <v>412</v>
+      </c>
+      <c r="C10" s="5" t="s">
         <v>22</v>
       </c>
-      <c r="D10" s="12" t="s">
+      <c r="D10" s="8">
+        <v>7798013100246</v>
+      </c>
+    </row>
+    <row r="11" spans="1:16">
+      <c r="A11" s="5">
+        <v>193</v>
+      </c>
+      <c r="B11" s="5">
+        <v>414</v>
+      </c>
+      <c r="C11" s="5" t="s">
         <v>23</v>
       </c>
-    </row>
-    <row r="11">
-      <c r="A11" s="9">
-        <v>193.0</v>
-      </c>
-      <c r="B11" s="9">
-        <v>414.0</v>
-      </c>
-      <c r="C11" s="9" t="s">
+      <c r="I11" s="8">
+        <v>2017139000007</v>
+      </c>
+    </row>
+    <row r="12" spans="1:16">
+      <c r="A12" s="5">
+        <v>199</v>
+      </c>
+      <c r="B12" s="5">
+        <v>420</v>
+      </c>
+      <c r="C12" s="5" t="s">
         <v>24</v>
       </c>
-      <c r="I11" s="12">
-        <v>2.017139000007E12</v>
-      </c>
-    </row>
-    <row r="12">
-      <c r="A12" s="9">
-        <v>199.0</v>
-      </c>
-      <c r="B12" s="9">
-        <v>420.0</v>
-      </c>
-      <c r="C12" s="9" t="s">
+      <c r="D12" s="8">
+        <v>2524469000008</v>
+      </c>
+    </row>
+    <row r="13" spans="1:16">
+      <c r="A13" s="5">
+        <v>1000</v>
+      </c>
+      <c r="B13" s="5">
+        <v>830</v>
+      </c>
+      <c r="C13" s="5" t="s">
         <v>25</v>
       </c>
-      <c r="D12" s="12">
-        <v>2.524469000008E12</v>
-      </c>
-    </row>
-    <row r="13">
-      <c r="A13" s="9">
-        <v>1000.0</v>
-      </c>
-      <c r="B13" s="9">
-        <v>830.0</v>
-      </c>
-      <c r="C13" s="9" t="s">
+    </row>
+    <row r="14" spans="1:16">
+      <c r="A14" s="5">
+        <v>252</v>
+      </c>
+      <c r="B14" s="5">
+        <v>874</v>
+      </c>
+      <c r="C14" s="5" t="s">
         <v>26</v>
       </c>
     </row>
-    <row r="14">
-      <c r="A14" s="9">
-        <v>252.0</v>
-      </c>
-      <c r="B14" s="9">
-        <v>874.0</v>
-      </c>
-      <c r="C14" s="9" t="s">
+    <row r="15" spans="1:16">
+      <c r="A15" s="5">
+        <v>234</v>
+      </c>
+      <c r="B15" s="5">
+        <v>1803</v>
+      </c>
+      <c r="C15" s="5" t="s">
         <v>27</v>
       </c>
     </row>
-    <row r="15">
-      <c r="A15" s="9">
-        <v>234.0</v>
-      </c>
-      <c r="B15" s="9">
-        <v>1803.0</v>
-      </c>
-      <c r="C15" s="9" t="s">
+    <row r="16" spans="1:16">
+      <c r="A16" s="5">
+        <v>235</v>
+      </c>
+      <c r="B16" s="5">
+        <v>1804</v>
+      </c>
+      <c r="C16" s="5" t="s">
         <v>28</v>
       </c>
-    </row>
-    <row r="16">
-      <c r="A16" s="9">
-        <v>235.0</v>
-      </c>
-      <c r="B16" s="9">
-        <v>1804.0</v>
-      </c>
-      <c r="C16" s="9" t="s">
+      <c r="D16" s="8">
+        <v>7798013100697</v>
+      </c>
+      <c r="I16" s="8">
+        <v>8428204012018</v>
+      </c>
+    </row>
+    <row r="17" spans="1:9">
+      <c r="A17" s="5">
+        <v>248</v>
+      </c>
+      <c r="B17" s="5">
+        <v>2664</v>
+      </c>
+      <c r="C17" s="5" t="s">
         <v>29</v>
       </c>
-      <c r="D16" s="12">
-        <v>7.798013100697E12</v>
-      </c>
-      <c r="I16" s="12">
-        <v>8.428204012018E12</v>
-      </c>
-    </row>
-    <row r="17">
-      <c r="A17" s="9">
-        <v>248.0</v>
-      </c>
-      <c r="B17" s="9">
-        <v>2664.0</v>
-      </c>
-      <c r="C17" s="9" t="s">
+      <c r="D17" s="8">
+        <v>2003796400007</v>
+      </c>
+    </row>
+    <row r="18" spans="1:9">
+      <c r="A18" s="5">
+        <v>249</v>
+      </c>
+      <c r="B18" s="5">
+        <v>2665</v>
+      </c>
+      <c r="C18" s="5" t="s">
         <v>30</v>
       </c>
-      <c r="D17" s="12">
-        <v>2.003796400007E12</v>
-      </c>
-    </row>
-    <row r="18">
-      <c r="A18" s="9">
-        <v>249.0</v>
-      </c>
-      <c r="B18" s="9">
-        <v>2665.0</v>
-      </c>
-      <c r="C18" s="9" t="s">
+      <c r="D18" s="8">
+        <v>2533120000004</v>
+      </c>
+    </row>
+    <row r="19" spans="1:9">
+      <c r="A19" s="5">
+        <v>262</v>
+      </c>
+      <c r="B19" s="5">
+        <v>2726</v>
+      </c>
+      <c r="C19" s="5" t="s">
         <v>31</v>
       </c>
-      <c r="D18" s="12">
-        <v>2.533120000004E12</v>
-      </c>
-    </row>
-    <row r="19">
-      <c r="A19" s="9">
-        <v>262.0</v>
-      </c>
-      <c r="B19" s="9">
-        <v>2726.0</v>
-      </c>
-      <c r="C19" s="9" t="s">
+    </row>
+    <row r="20" spans="1:9">
+      <c r="A20" s="5">
+        <v>263</v>
+      </c>
+      <c r="B20" s="5">
+        <v>2727</v>
+      </c>
+      <c r="C20" s="5" t="s">
         <v>32</v>
       </c>
     </row>
-    <row r="20">
-      <c r="A20" s="9">
-        <v>263.0</v>
-      </c>
-      <c r="B20" s="9">
-        <v>2727.0</v>
-      </c>
-      <c r="C20" s="9" t="s">
+    <row r="21" spans="1:9" ht="15.75" customHeight="1">
+      <c r="A21" s="5">
+        <v>267</v>
+      </c>
+      <c r="B21" s="5">
+        <v>2763</v>
+      </c>
+      <c r="C21" s="5" t="s">
         <v>33</v>
       </c>
     </row>
-    <row r="21" ht="15.75" customHeight="1">
-      <c r="A21" s="9">
-        <v>267.0</v>
-      </c>
-      <c r="B21" s="9">
-        <v>2763.0</v>
-      </c>
-      <c r="C21" s="9" t="s">
+    <row r="22" spans="1:9" ht="15.75" customHeight="1">
+      <c r="A22" s="5">
+        <v>287</v>
+      </c>
+      <c r="B22" s="5">
+        <v>3347</v>
+      </c>
+      <c r="C22" s="5" t="s">
         <v>34</v>
       </c>
     </row>
-    <row r="22" ht="15.75" customHeight="1">
-      <c r="A22" s="9">
-        <v>287.0</v>
-      </c>
-      <c r="B22" s="9">
-        <v>3347.0</v>
-      </c>
-      <c r="C22" s="9" t="s">
+    <row r="23" spans="1:9" ht="15.75" customHeight="1">
+      <c r="A23" s="5">
+        <v>250</v>
+      </c>
+      <c r="B23" s="5">
+        <v>4946</v>
+      </c>
+      <c r="C23" s="5" t="s">
         <v>35</v>
       </c>
     </row>
-    <row r="23" ht="15.75" customHeight="1">
-      <c r="A23" s="9">
-        <v>250.0</v>
-      </c>
-      <c r="B23" s="9">
-        <v>4946.0</v>
-      </c>
-      <c r="C23" s="9" t="s">
+    <row r="24" spans="1:9" ht="15.75" customHeight="1">
+      <c r="A24" s="5">
+        <v>251</v>
+      </c>
+      <c r="B24" s="5">
+        <v>4947</v>
+      </c>
+      <c r="C24" s="5" t="s">
         <v>36</v>
       </c>
     </row>
-    <row r="24" ht="15.75" customHeight="1">
-      <c r="A24" s="9">
-        <v>251.0</v>
-      </c>
-      <c r="B24" s="9">
-        <v>4947.0</v>
-      </c>
-      <c r="C24" s="9" t="s">
+    <row r="25" spans="1:9" ht="15.75" customHeight="1">
+      <c r="A25" s="5">
+        <v>308</v>
+      </c>
+      <c r="B25" s="5">
+        <v>5574</v>
+      </c>
+      <c r="C25" s="5" t="s">
         <v>37</v>
       </c>
-    </row>
-    <row r="25" ht="15.75" customHeight="1">
-      <c r="A25" s="9">
-        <v>308.0</v>
-      </c>
-      <c r="B25" s="9">
-        <v>5574.0</v>
-      </c>
-      <c r="C25" s="9" t="s">
+      <c r="H25" s="7" t="s">
         <v>38</v>
       </c>
-      <c r="H25" s="11" t="s">
+      <c r="I25" s="8">
+        <v>2009380000004</v>
+      </c>
+    </row>
+    <row r="26" spans="1:9" ht="15.75" customHeight="1">
+      <c r="A26" s="5">
+        <v>33</v>
+      </c>
+      <c r="B26" s="5">
+        <v>41</v>
+      </c>
+      <c r="C26" s="5" t="s">
         <v>39</v>
       </c>
-      <c r="I25" s="12" t="s">
+      <c r="D26" s="8">
+        <v>7798013107726</v>
+      </c>
+      <c r="H26" s="8">
+        <v>7798183684102</v>
+      </c>
+      <c r="I26" s="8">
+        <v>2000000132877</v>
+      </c>
+    </row>
+    <row r="27" spans="1:9" ht="15.75" customHeight="1">
+      <c r="A27" s="5">
+        <v>34</v>
+      </c>
+      <c r="B27" s="5">
+        <v>42</v>
+      </c>
+      <c r="C27" s="5" t="s">
         <v>40</v>
       </c>
-    </row>
-    <row r="26" ht="15.75" customHeight="1">
-      <c r="A26" s="9">
-        <v>33.0</v>
-      </c>
-      <c r="B26" s="9">
-        <v>41.0</v>
-      </c>
-      <c r="C26" s="9" t="s">
+      <c r="I27" s="8"/>
+    </row>
+    <row r="28" spans="1:9" ht="15.75" customHeight="1">
+      <c r="A28" s="5">
+        <v>98</v>
+      </c>
+      <c r="B28" s="5">
+        <v>150</v>
+      </c>
+      <c r="C28" s="5" t="s">
         <v>41</v>
       </c>
-      <c r="D26" s="12" t="s">
+    </row>
+    <row r="29" spans="1:9" ht="15.75" customHeight="1">
+      <c r="A29" s="5">
+        <v>134</v>
+      </c>
+      <c r="B29" s="5">
+        <v>197</v>
+      </c>
+      <c r="C29" s="5" t="s">
         <v>42</v>
       </c>
-      <c r="H26" s="12" t="s">
+    </row>
+    <row r="30" spans="1:9" ht="15.75" customHeight="1">
+      <c r="A30" s="5">
+        <v>202</v>
+      </c>
+      <c r="B30" s="5">
+        <v>426</v>
+      </c>
+      <c r="C30" s="5" t="s">
         <v>43</v>
       </c>
-      <c r="I26" s="12">
-        <v>2.000000132877E12</v>
-      </c>
-    </row>
-    <row r="27" ht="15.75" customHeight="1">
-      <c r="A27" s="9">
-        <v>34.0</v>
-      </c>
-      <c r="B27" s="9">
-        <v>42.0</v>
-      </c>
-      <c r="C27" s="9" t="s">
+      <c r="I30" s="8">
+        <v>2034894000004</v>
+      </c>
+    </row>
+    <row r="31" spans="1:9" ht="15.75" customHeight="1">
+      <c r="A31" s="5">
+        <v>258</v>
+      </c>
+      <c r="B31" s="5">
+        <v>2709</v>
+      </c>
+      <c r="C31" s="5" t="s">
         <v>44</v>
       </c>
-      <c r="I27" s="12"/>
-    </row>
-    <row r="28" ht="15.75" customHeight="1">
-      <c r="A28" s="9">
-        <v>98.0</v>
-      </c>
-      <c r="B28" s="9">
-        <v>150.0</v>
-      </c>
-      <c r="C28" s="9" t="s">
+    </row>
+    <row r="32" spans="1:9" ht="15.75" customHeight="1">
+      <c r="A32" s="5">
+        <v>292</v>
+      </c>
+      <c r="B32" s="5">
+        <v>5635</v>
+      </c>
+      <c r="C32" s="5" t="s">
         <v>45</v>
       </c>
     </row>
-    <row r="29" ht="15.75" customHeight="1">
-      <c r="A29" s="9">
-        <v>134.0</v>
-      </c>
-      <c r="B29" s="9">
-        <v>197.0</v>
-      </c>
-      <c r="C29" s="9" t="s">
+    <row r="33" spans="1:9" ht="15.75" customHeight="1">
+      <c r="A33" s="5">
+        <v>79</v>
+      </c>
+      <c r="B33" s="5">
+        <v>129</v>
+      </c>
+      <c r="C33" s="5" t="s">
         <v>46</v>
       </c>
     </row>
-    <row r="30" ht="15.75" customHeight="1">
-      <c r="A30" s="9">
-        <v>202.0</v>
-      </c>
-      <c r="B30" s="9">
-        <v>426.0</v>
-      </c>
-      <c r="C30" s="9" t="s">
+    <row r="34" spans="1:9" ht="15.75" customHeight="1">
+      <c r="A34" s="5">
+        <v>150</v>
+      </c>
+      <c r="B34" s="5">
+        <v>246</v>
+      </c>
+      <c r="C34" s="5" t="s">
         <v>47</v>
       </c>
-      <c r="I30" s="12">
-        <v>2.034894000004E12</v>
-      </c>
-    </row>
-    <row r="31" ht="15.75" customHeight="1">
-      <c r="A31" s="9">
-        <v>258.0</v>
-      </c>
-      <c r="B31" s="9">
-        <v>2709.0</v>
-      </c>
-      <c r="C31" s="9" t="s">
+    </row>
+    <row r="35" spans="1:9" ht="15.75" customHeight="1">
+      <c r="A35" s="5">
+        <v>160</v>
+      </c>
+      <c r="B35" s="5">
+        <v>297</v>
+      </c>
+      <c r="C35" s="5" t="s">
         <v>48</v>
       </c>
     </row>
-    <row r="32" ht="15.75" customHeight="1">
-      <c r="A32" s="9">
-        <v>292.0</v>
-      </c>
-      <c r="B32" s="9">
-        <v>5635.0</v>
-      </c>
-      <c r="C32" s="9" t="s">
+    <row r="36" spans="1:9" ht="15.75" customHeight="1">
+      <c r="A36" s="5">
+        <v>171</v>
+      </c>
+      <c r="B36" s="5">
+        <v>1091</v>
+      </c>
+      <c r="C36" s="5" t="s">
         <v>49</v>
       </c>
     </row>
-    <row r="33" ht="15.75" customHeight="1">
-      <c r="A33" s="9">
-        <v>79.0</v>
-      </c>
-      <c r="B33" s="9">
-        <v>129.0</v>
-      </c>
-      <c r="C33" s="9" t="s">
+    <row r="37" spans="1:9" ht="15.75" customHeight="1">
+      <c r="A37" s="5">
+        <v>174</v>
+      </c>
+      <c r="B37" s="5">
+        <v>1133</v>
+      </c>
+      <c r="C37" s="5" t="s">
         <v>50</v>
       </c>
     </row>
-    <row r="34" ht="15.75" customHeight="1">
-      <c r="A34" s="9">
-        <v>150.0</v>
-      </c>
-      <c r="B34" s="9">
-        <v>246.0</v>
-      </c>
-      <c r="C34" s="9" t="s">
+    <row r="38" spans="1:9" ht="15.75" customHeight="1">
+      <c r="A38" s="5">
+        <v>106</v>
+      </c>
+      <c r="B38" s="5">
+        <v>161</v>
+      </c>
+      <c r="C38" s="5" t="s">
         <v>51</v>
       </c>
-    </row>
-    <row r="35" ht="15.75" customHeight="1">
-      <c r="A35" s="9">
-        <v>160.0</v>
-      </c>
-      <c r="B35" s="9">
-        <v>297.0</v>
-      </c>
-      <c r="C35" s="9" t="s">
+      <c r="G38" s="8">
+        <v>2000000160696</v>
+      </c>
+    </row>
+    <row r="39" spans="1:9" ht="15.75" customHeight="1">
+      <c r="A39" s="5">
+        <v>121</v>
+      </c>
+      <c r="B39" s="5">
+        <v>180</v>
+      </c>
+      <c r="C39" s="5" t="s">
         <v>52</v>
       </c>
-    </row>
-    <row r="36" ht="15.75" customHeight="1">
-      <c r="A36" s="9">
-        <v>171.0</v>
-      </c>
-      <c r="B36" s="9">
-        <v>1091.0</v>
-      </c>
-      <c r="C36" s="9" t="s">
+      <c r="G39" s="8">
+        <v>2000000184630</v>
+      </c>
+      <c r="I39" s="8">
+        <v>2303127000006</v>
+      </c>
+    </row>
+    <row r="40" spans="1:9" ht="15.75" customHeight="1">
+      <c r="A40" s="5">
+        <v>125</v>
+      </c>
+      <c r="B40" s="5">
+        <v>184</v>
+      </c>
+      <c r="C40" s="5" t="s">
         <v>53</v>
       </c>
-    </row>
-    <row r="37" ht="15.75" customHeight="1">
-      <c r="A37" s="9">
-        <v>174.0</v>
-      </c>
-      <c r="B37" s="9">
-        <v>1133.0</v>
-      </c>
-      <c r="C37" s="9" t="s">
+      <c r="D40" s="8">
+        <v>2567634000007</v>
+      </c>
+      <c r="I40" s="8">
+        <v>2530470000005</v>
+      </c>
+    </row>
+    <row r="41" spans="1:9" ht="15.75" customHeight="1">
+      <c r="A41" s="5">
+        <v>130</v>
+      </c>
+      <c r="B41" s="5">
+        <v>189</v>
+      </c>
+      <c r="C41" s="5" t="s">
         <v>54</v>
       </c>
     </row>
-    <row r="38" ht="15.75" customHeight="1">
-      <c r="A38" s="9">
-        <v>106.0</v>
-      </c>
-      <c r="B38" s="9">
-        <v>161.0</v>
-      </c>
-      <c r="C38" s="9" t="s">
+    <row r="42" spans="1:9" ht="15.75" customHeight="1">
+      <c r="A42" s="5">
+        <v>133</v>
+      </c>
+      <c r="B42" s="5">
+        <v>196</v>
+      </c>
+      <c r="C42" s="5" t="s">
         <v>55</v>
       </c>
-      <c r="G38" s="12">
-        <v>2.000000160696E12</v>
-      </c>
-    </row>
-    <row r="39" ht="15.75" customHeight="1">
-      <c r="A39" s="9">
-        <v>121.0</v>
-      </c>
-      <c r="B39" s="9">
-        <v>180.0</v>
-      </c>
-      <c r="C39" s="9" t="s">
+      <c r="G42" s="8">
+        <v>2000000160924</v>
+      </c>
+      <c r="I42" s="8">
+        <v>2305927000002</v>
+      </c>
+    </row>
+    <row r="43" spans="1:9" ht="15.75" customHeight="1">
+      <c r="A43" s="5">
+        <v>138</v>
+      </c>
+      <c r="B43" s="5">
+        <v>202</v>
+      </c>
+      <c r="C43" s="5" t="s">
         <v>56</v>
       </c>
-      <c r="G39" s="12">
-        <v>2.00000018463E12</v>
-      </c>
-      <c r="I39" s="12">
-        <v>2.303127000006E12</v>
-      </c>
-    </row>
-    <row r="40" ht="15.75" customHeight="1">
-      <c r="A40" s="9">
-        <v>125.0</v>
-      </c>
-      <c r="B40" s="9">
-        <v>184.0</v>
-      </c>
-      <c r="C40" s="9" t="s">
+      <c r="H43" s="8">
+        <v>7798183683556</v>
+      </c>
+    </row>
+    <row r="44" spans="1:9" ht="15.75" customHeight="1">
+      <c r="A44" s="5">
+        <v>192</v>
+      </c>
+      <c r="B44" s="5">
+        <v>413</v>
+      </c>
+      <c r="C44" s="5" t="s">
         <v>57</v>
       </c>
-      <c r="D40" s="12">
-        <v>2.567634000007E12</v>
-      </c>
-      <c r="I40" s="12">
-        <v>2.530470000005E12</v>
-      </c>
-    </row>
-    <row r="41" ht="15.75" customHeight="1">
-      <c r="A41" s="9">
-        <v>130.0</v>
-      </c>
-      <c r="B41" s="9">
-        <v>189.0</v>
-      </c>
-      <c r="C41" s="9" t="s">
+      <c r="D44" s="8">
+        <v>2555479000009</v>
+      </c>
+    </row>
+    <row r="45" spans="1:9" ht="15.75" customHeight="1">
+      <c r="A45" s="5">
+        <v>195</v>
+      </c>
+      <c r="B45" s="5">
+        <v>416</v>
+      </c>
+      <c r="C45" s="5" t="s">
         <v>58</v>
       </c>
-    </row>
-    <row r="42" ht="15.75" customHeight="1">
-      <c r="A42" s="9">
-        <v>133.0</v>
-      </c>
-      <c r="B42" s="9">
-        <v>196.0</v>
-      </c>
-      <c r="C42" s="9" t="s">
+      <c r="D45" s="8">
+        <v>2567634000007</v>
+      </c>
+      <c r="I45" s="8">
+        <v>2530470000005</v>
+      </c>
+    </row>
+    <row r="46" spans="1:9" ht="15.75" customHeight="1">
+      <c r="A46" s="5">
+        <v>201</v>
+      </c>
+      <c r="B46" s="5">
+        <v>425</v>
+      </c>
+      <c r="C46" s="5" t="s">
         <v>59</v>
       </c>
-      <c r="G42" s="12">
-        <v>2.000000160924E12</v>
-      </c>
-      <c r="I42" s="12">
-        <v>2.305927000002E12</v>
-      </c>
-    </row>
-    <row r="43" ht="15.75" customHeight="1">
-      <c r="A43" s="9">
-        <v>138.0</v>
-      </c>
-      <c r="B43" s="9">
-        <v>202.0</v>
-      </c>
-      <c r="C43" s="9" t="s">
+      <c r="I46" s="8">
+        <v>2303521000008</v>
+      </c>
+    </row>
+    <row r="47" spans="1:9" ht="15.75" customHeight="1">
+      <c r="A47" s="5">
+        <v>203</v>
+      </c>
+      <c r="B47" s="5">
+        <v>462</v>
+      </c>
+      <c r="C47" s="5" t="s">
         <v>60</v>
       </c>
-      <c r="H43" s="12" t="s">
+      <c r="I47" s="8">
+        <v>7790079019913</v>
+      </c>
+    </row>
+    <row r="48" spans="1:9" ht="15.75" customHeight="1">
+      <c r="A48" s="5">
+        <v>228</v>
+      </c>
+      <c r="B48" s="5">
+        <v>711</v>
+      </c>
+      <c r="C48" s="5" t="s">
         <v>61</v>
       </c>
     </row>
-    <row r="44" ht="15.75" customHeight="1">
-      <c r="A44" s="9">
-        <v>192.0</v>
-      </c>
-      <c r="B44" s="9">
-        <v>413.0</v>
-      </c>
-      <c r="C44" s="9" t="s">
+    <row r="49" spans="1:9" ht="15.75" customHeight="1">
+      <c r="A49" s="5">
+        <v>231</v>
+      </c>
+      <c r="B49" s="5">
+        <v>714</v>
+      </c>
+      <c r="C49" s="5" t="s">
         <v>62</v>
       </c>
-      <c r="D44" s="12">
-        <v>2.555479000009E12</v>
-      </c>
-    </row>
-    <row r="45" ht="15.75" customHeight="1">
-      <c r="A45" s="9">
-        <v>195.0</v>
-      </c>
-      <c r="B45" s="9">
-        <v>416.0</v>
-      </c>
-      <c r="C45" s="9" t="s">
+    </row>
+    <row r="50" spans="1:9" ht="15.75" customHeight="1">
+      <c r="A50" s="5">
+        <v>237</v>
+      </c>
+      <c r="B50" s="5">
+        <v>717</v>
+      </c>
+      <c r="C50" s="5" t="s">
         <v>63</v>
       </c>
-      <c r="D45" s="12">
-        <v>2.567634000007E12</v>
-      </c>
-      <c r="I45" s="12">
-        <v>2.530470000005E12</v>
-      </c>
-    </row>
-    <row r="46" ht="15.75" customHeight="1">
-      <c r="A46" s="9">
-        <v>201.0</v>
-      </c>
-      <c r="B46" s="9">
-        <v>425.0</v>
-      </c>
-      <c r="C46" s="9" t="s">
+      <c r="G50" s="8">
+        <v>2000000160672</v>
+      </c>
+      <c r="I50" s="8">
+        <v>2000000471075</v>
+      </c>
+    </row>
+    <row r="51" spans="1:9" ht="15.75" customHeight="1">
+      <c r="A51" s="5">
+        <v>245</v>
+      </c>
+      <c r="B51" s="5">
+        <v>2210</v>
+      </c>
+      <c r="C51" s="5" t="s">
         <v>64</v>
       </c>
-      <c r="I46" s="12">
-        <v>2.303521000008E12</v>
-      </c>
-    </row>
-    <row r="47" ht="15.75" customHeight="1">
-      <c r="A47" s="9">
-        <v>203.0</v>
-      </c>
-      <c r="B47" s="9">
-        <v>462.0</v>
-      </c>
-      <c r="C47" s="9" t="s">
+    </row>
+    <row r="52" spans="1:9" ht="15.75" customHeight="1">
+      <c r="A52" s="5">
+        <v>178</v>
+      </c>
+      <c r="B52" s="5">
+        <v>2380</v>
+      </c>
+      <c r="C52" s="5" t="s">
         <v>65</v>
       </c>
-      <c r="I47" s="12" t="s">
+      <c r="I52" s="8">
+        <v>2508447000006</v>
+      </c>
+    </row>
+    <row r="53" spans="1:9" ht="15.75" customHeight="1">
+      <c r="A53" s="5">
+        <v>179</v>
+      </c>
+      <c r="B53" s="5">
+        <v>2381</v>
+      </c>
+      <c r="C53" s="5" t="s">
         <v>66</v>
       </c>
-    </row>
-    <row r="48" ht="15.75" customHeight="1">
-      <c r="A48" s="9">
-        <v>228.0</v>
-      </c>
-      <c r="B48" s="9">
-        <v>711.0</v>
-      </c>
-      <c r="C48" s="9" t="s">
+      <c r="I53" s="8">
+        <v>2525851000002</v>
+      </c>
+    </row>
+    <row r="54" spans="1:9" ht="15.75" customHeight="1">
+      <c r="A54" s="5">
+        <v>305</v>
+      </c>
+      <c r="B54" s="5">
+        <v>2422</v>
+      </c>
+      <c r="C54" s="5" t="s">
         <v>67</v>
       </c>
-    </row>
-    <row r="49" ht="15.75" customHeight="1">
-      <c r="A49" s="9">
-        <v>231.0</v>
-      </c>
-      <c r="B49" s="9">
-        <v>714.0</v>
-      </c>
-      <c r="C49" s="9" t="s">
+      <c r="I54" s="8">
+        <v>2506598000005</v>
+      </c>
+    </row>
+    <row r="55" spans="1:9" ht="15.75" customHeight="1">
+      <c r="A55" s="5">
+        <v>306</v>
+      </c>
+      <c r="B55" s="5">
+        <v>2423</v>
+      </c>
+      <c r="C55" s="5" t="s">
         <v>68</v>
       </c>
-    </row>
-    <row r="50" ht="15.75" customHeight="1">
-      <c r="A50" s="9">
-        <v>237.0</v>
-      </c>
-      <c r="B50" s="9">
-        <v>717.0</v>
-      </c>
-      <c r="C50" s="9" t="s">
+      <c r="I55" s="8">
+        <v>2595324000006</v>
+      </c>
+    </row>
+    <row r="56" spans="1:9" ht="15.75" customHeight="1">
+      <c r="A56" s="5">
+        <v>247</v>
+      </c>
+      <c r="B56" s="5">
+        <v>2475</v>
+      </c>
+      <c r="C56" s="5" t="s">
         <v>69</v>
       </c>
-      <c r="G50" s="12">
-        <v>2.000000160672E12</v>
-      </c>
-      <c r="I50" s="12">
-        <v>2.000000471075E12</v>
-      </c>
-    </row>
-    <row r="51" ht="15.75" customHeight="1">
-      <c r="A51" s="9">
-        <v>245.0</v>
-      </c>
-      <c r="B51" s="9">
-        <v>2210.0</v>
-      </c>
-      <c r="C51" s="9" t="s">
+      <c r="I56" s="8">
+        <v>2508691000005</v>
+      </c>
+    </row>
+    <row r="57" spans="1:9" ht="15.75" customHeight="1">
+      <c r="A57" s="5">
+        <v>246</v>
+      </c>
+      <c r="B57" s="5">
+        <v>2476</v>
+      </c>
+      <c r="C57" s="5" t="s">
         <v>70</v>
       </c>
     </row>
-    <row r="52" ht="15.75" customHeight="1">
-      <c r="A52" s="9">
-        <v>178.0</v>
-      </c>
-      <c r="B52" s="9">
-        <v>2380.0</v>
-      </c>
-      <c r="C52" s="9" t="s">
+    <row r="58" spans="1:9" ht="15.75" customHeight="1">
+      <c r="A58" s="5">
+        <v>230</v>
+      </c>
+      <c r="B58" s="5">
+        <v>4709</v>
+      </c>
+      <c r="C58" s="5" t="s">
         <v>71</v>
       </c>
-      <c r="I52" s="12">
-        <v>2.508447000006E12</v>
-      </c>
-    </row>
-    <row r="53" ht="15.75" customHeight="1">
-      <c r="A53" s="9">
-        <v>179.0</v>
-      </c>
-      <c r="B53" s="9">
-        <v>2381.0</v>
-      </c>
-      <c r="C53" s="9" t="s">
+    </row>
+    <row r="59" spans="1:9" ht="15.75" customHeight="1">
+      <c r="A59" s="5">
+        <v>58</v>
+      </c>
+      <c r="B59" s="5">
+        <v>108</v>
+      </c>
+      <c r="C59" s="5" t="s">
         <v>72</v>
       </c>
-      <c r="I53" s="12">
-        <v>2.525851000002E12</v>
-      </c>
-    </row>
-    <row r="54" ht="15.75" customHeight="1">
-      <c r="A54" s="9">
-        <v>305.0</v>
-      </c>
-      <c r="B54" s="9">
-        <v>2422.0</v>
-      </c>
-      <c r="C54" s="9" t="s">
+      <c r="I59" s="8">
+        <v>2507571000005</v>
+      </c>
+    </row>
+    <row r="60" spans="1:9" ht="15.75" customHeight="1">
+      <c r="A60" s="5">
+        <v>60</v>
+      </c>
+      <c r="B60" s="5">
+        <v>110</v>
+      </c>
+      <c r="C60" s="5" t="s">
         <v>73</v>
       </c>
-      <c r="I54" s="12">
-        <v>2.506598000005E12</v>
-      </c>
-    </row>
-    <row r="55" ht="15.75" customHeight="1">
-      <c r="A55" s="9">
-        <v>306.0</v>
-      </c>
-      <c r="B55" s="9">
-        <v>2423.0</v>
-      </c>
-      <c r="C55" s="9" t="s">
+      <c r="I60" s="8">
+        <v>2000943000004</v>
+      </c>
+    </row>
+    <row r="61" spans="1:9" ht="15.75" customHeight="1">
+      <c r="A61" s="5">
+        <v>61</v>
+      </c>
+      <c r="B61" s="5">
+        <v>111</v>
+      </c>
+      <c r="C61" s="5" t="s">
         <v>74</v>
       </c>
-      <c r="I55" s="12">
-        <v>2.595324000006E12</v>
-      </c>
-    </row>
-    <row r="56" ht="15.75" customHeight="1">
-      <c r="A56" s="9">
-        <v>247.0</v>
-      </c>
-      <c r="B56" s="9">
-        <v>2475.0</v>
-      </c>
-      <c r="C56" s="9" t="s">
+      <c r="I61" s="8">
+        <v>2034913000008</v>
+      </c>
+    </row>
+    <row r="62" spans="1:9" ht="15.75" customHeight="1">
+      <c r="A62" s="5">
+        <v>62</v>
+      </c>
+      <c r="B62" s="5">
+        <v>112</v>
+      </c>
+      <c r="C62" s="5" t="s">
         <v>75</v>
       </c>
-      <c r="I56" s="12">
-        <v>2.508691000005E12</v>
-      </c>
-    </row>
-    <row r="57" ht="15.75" customHeight="1">
-      <c r="A57" s="9">
-        <v>246.0</v>
-      </c>
-      <c r="B57" s="9">
-        <v>2476.0</v>
-      </c>
-      <c r="C57" s="9" t="s">
+    </row>
+    <row r="63" spans="1:9" ht="15.75" customHeight="1">
+      <c r="A63" s="5">
+        <v>71</v>
+      </c>
+      <c r="B63" s="5">
+        <v>121</v>
+      </c>
+      <c r="C63" s="5" t="s">
         <v>76</v>
       </c>
-    </row>
-    <row r="58" ht="15.75" customHeight="1">
-      <c r="A58" s="9">
-        <v>230.0</v>
-      </c>
-      <c r="B58" s="9">
-        <v>4709.0</v>
-      </c>
-      <c r="C58" s="9" t="s">
+      <c r="G63" s="8">
+        <v>2000000184685</v>
+      </c>
+    </row>
+    <row r="64" spans="1:9" ht="15.75" customHeight="1">
+      <c r="A64" s="5">
+        <v>91</v>
+      </c>
+      <c r="B64" s="5">
+        <v>143</v>
+      </c>
+      <c r="C64" s="5" t="s">
         <v>77</v>
       </c>
     </row>
-    <row r="59" ht="15.75" customHeight="1">
-      <c r="A59" s="9">
-        <v>58.0</v>
-      </c>
-      <c r="B59" s="9">
-        <v>108.0</v>
-      </c>
-      <c r="C59" s="9" t="s">
+    <row r="65" spans="1:9" ht="15.75" customHeight="1">
+      <c r="A65" s="5">
+        <v>151</v>
+      </c>
+      <c r="B65" s="5">
+        <v>256</v>
+      </c>
+      <c r="C65" s="5" t="s">
         <v>78</v>
       </c>
-      <c r="I59" s="12">
-        <v>2.507571000005E12</v>
-      </c>
-    </row>
-    <row r="60" ht="15.75" customHeight="1">
-      <c r="A60" s="9">
-        <v>60.0</v>
-      </c>
-      <c r="B60" s="9">
-        <v>110.0</v>
-      </c>
-      <c r="C60" s="9" t="s">
+    </row>
+    <row r="66" spans="1:9" ht="15.75" customHeight="1">
+      <c r="A66" s="5">
+        <v>152</v>
+      </c>
+      <c r="B66" s="5">
+        <v>257</v>
+      </c>
+      <c r="C66" s="5" t="s">
         <v>79</v>
       </c>
-      <c r="I60" s="12">
-        <v>2.000943000004E12</v>
-      </c>
-    </row>
-    <row r="61" ht="15.75" customHeight="1">
-      <c r="A61" s="9">
-        <v>61.0</v>
-      </c>
-      <c r="B61" s="9">
-        <v>111.0</v>
-      </c>
-      <c r="C61" s="9" t="s">
+      <c r="I66" s="8">
+        <v>7798016105668</v>
+      </c>
+    </row>
+    <row r="67" spans="1:9" ht="15.75" customHeight="1">
+      <c r="A67" s="5">
+        <v>200</v>
+      </c>
+      <c r="B67" s="5">
+        <v>421</v>
+      </c>
+      <c r="C67" s="5" t="s">
         <v>80</v>
       </c>
-      <c r="I61" s="12">
-        <v>2.034913000008E12</v>
-      </c>
-    </row>
-    <row r="62" ht="15.75" customHeight="1">
-      <c r="A62" s="9">
-        <v>62.0</v>
-      </c>
-      <c r="B62" s="9">
-        <v>112.0</v>
-      </c>
-      <c r="C62" s="9" t="s">
+      <c r="I67" s="8">
+        <v>7790079016295</v>
+      </c>
+    </row>
+    <row r="68" spans="1:9" ht="15.75" customHeight="1">
+      <c r="A68" s="5">
+        <v>180</v>
+      </c>
+      <c r="B68" s="5">
+        <v>858</v>
+      </c>
+      <c r="C68" s="5" t="s">
         <v>81</v>
       </c>
-    </row>
-    <row r="63" ht="15.75" customHeight="1">
-      <c r="A63" s="9">
-        <v>71.0</v>
-      </c>
-      <c r="B63" s="9">
-        <v>121.0</v>
-      </c>
-      <c r="C63" s="9" t="s">
+      <c r="D68" s="8"/>
+      <c r="G68" s="8"/>
+    </row>
+    <row r="69" spans="1:9" ht="15.75" customHeight="1">
+      <c r="A69" s="5">
+        <v>181</v>
+      </c>
+      <c r="B69" s="5">
+        <v>859</v>
+      </c>
+      <c r="C69" s="5" t="s">
         <v>82</v>
       </c>
-      <c r="G63" s="12">
-        <v>2.000000184685E12</v>
-      </c>
-    </row>
-    <row r="64" ht="15.75" customHeight="1">
-      <c r="A64" s="9">
-        <v>91.0</v>
-      </c>
-      <c r="B64" s="9">
-        <v>143.0</v>
-      </c>
-      <c r="C64" s="9" t="s">
+      <c r="D69" s="8">
+        <v>2000000134604</v>
+      </c>
+      <c r="G69" s="8"/>
+    </row>
+    <row r="70" spans="1:9" ht="15.75" customHeight="1">
+      <c r="A70" s="5">
+        <v>182</v>
+      </c>
+      <c r="B70" s="5">
+        <v>860</v>
+      </c>
+      <c r="C70" s="5" t="s">
         <v>83</v>
       </c>
-    </row>
-    <row r="65" ht="15.75" customHeight="1">
-      <c r="A65" s="9">
-        <v>151.0</v>
-      </c>
-      <c r="B65" s="9">
-        <v>256.0</v>
-      </c>
-      <c r="C65" s="9" t="s">
+      <c r="D70" s="8"/>
+      <c r="G70" s="8"/>
+    </row>
+    <row r="71" spans="1:9" ht="15.75" customHeight="1">
+      <c r="A71" s="5">
+        <v>183</v>
+      </c>
+      <c r="B71" s="5">
+        <v>861</v>
+      </c>
+      <c r="C71" s="5" t="s">
         <v>84</v>
       </c>
-    </row>
-    <row r="66" ht="15.75" customHeight="1">
-      <c r="A66" s="9">
-        <v>152.0</v>
-      </c>
-      <c r="B66" s="9">
-        <v>257.0</v>
-      </c>
-      <c r="C66" s="9" t="s">
+      <c r="D71" s="8"/>
+      <c r="G71" s="8"/>
+    </row>
+    <row r="72" spans="1:9" ht="15.75" customHeight="1">
+      <c r="A72" s="5">
+        <v>184</v>
+      </c>
+      <c r="B72" s="5">
+        <v>862</v>
+      </c>
+      <c r="C72" s="5" t="s">
         <v>85</v>
       </c>
-      <c r="I66" s="12" t="s">
+      <c r="D72" s="8"/>
+      <c r="G72" s="8"/>
+    </row>
+    <row r="73" spans="1:9" ht="15.75" customHeight="1">
+      <c r="A73" s="5">
+        <v>185</v>
+      </c>
+      <c r="B73" s="5">
+        <v>863</v>
+      </c>
+      <c r="C73" s="5" t="s">
         <v>86</v>
       </c>
-    </row>
-    <row r="67" ht="15.75" customHeight="1">
-      <c r="A67" s="9">
-        <v>200.0</v>
-      </c>
-      <c r="B67" s="9">
-        <v>421.0</v>
-      </c>
-      <c r="C67" s="9" t="s">
+      <c r="D73" s="8"/>
+      <c r="G73" s="8"/>
+    </row>
+    <row r="74" spans="1:9" ht="15.75" customHeight="1">
+      <c r="A74" s="5">
+        <v>186</v>
+      </c>
+      <c r="B74" s="5">
+        <v>864</v>
+      </c>
+      <c r="C74" s="5" t="s">
         <v>87</v>
       </c>
-      <c r="I67" s="12">
-        <v>7.790079016295E12</v>
-      </c>
-    </row>
-    <row r="68" ht="15.75" customHeight="1">
-      <c r="A68" s="9">
-        <v>180.0</v>
-      </c>
-      <c r="B68" s="9">
-        <v>858.0</v>
-      </c>
-      <c r="C68" s="9" t="s">
+      <c r="D74" s="8"/>
+      <c r="G74" s="8">
+        <v>2000000184654</v>
+      </c>
+    </row>
+    <row r="75" spans="1:9" ht="15.75" customHeight="1">
+      <c r="A75" s="5">
+        <v>187</v>
+      </c>
+      <c r="B75" s="5">
+        <v>865</v>
+      </c>
+      <c r="C75" s="5" t="s">
         <v>88</v>
       </c>
-      <c r="D68" s="12"/>
-      <c r="G68" s="12"/>
-    </row>
-    <row r="69" ht="15.75" customHeight="1">
-      <c r="A69" s="9">
-        <v>181.0</v>
-      </c>
-      <c r="B69" s="9">
-        <v>859.0</v>
-      </c>
-      <c r="C69" s="9" t="s">
+      <c r="D75" s="8"/>
+      <c r="G75" s="8"/>
+    </row>
+    <row r="76" spans="1:9" ht="15.75" customHeight="1">
+      <c r="A76" s="5">
+        <v>188</v>
+      </c>
+      <c r="B76" s="5">
+        <v>991</v>
+      </c>
+      <c r="C76" s="5" t="s">
         <v>89</v>
       </c>
-      <c r="D69" s="12">
-        <v>2.000000134604E12</v>
-      </c>
-      <c r="G69" s="12"/>
-    </row>
-    <row r="70" ht="15.75" customHeight="1">
-      <c r="A70" s="9">
-        <v>182.0</v>
-      </c>
-      <c r="B70" s="9">
-        <v>860.0</v>
-      </c>
-      <c r="C70" s="9" t="s">
+      <c r="I76" s="8">
+        <v>2555477000001</v>
+      </c>
+    </row>
+    <row r="77" spans="1:9" ht="15.75" customHeight="1">
+      <c r="A77" s="5">
+        <v>189</v>
+      </c>
+      <c r="B77" s="5">
+        <v>1082</v>
+      </c>
+      <c r="C77" s="5" t="s">
         <v>90</v>
       </c>
-      <c r="D70" s="12"/>
-      <c r="G70" s="12"/>
-    </row>
-    <row r="71" ht="15.75" customHeight="1">
-      <c r="A71" s="9">
-        <v>183.0</v>
-      </c>
-      <c r="B71" s="9">
-        <v>861.0</v>
-      </c>
-      <c r="C71" s="9" t="s">
+    </row>
+    <row r="78" spans="1:9" ht="15.75" customHeight="1">
+      <c r="A78" s="5">
+        <v>244</v>
+      </c>
+      <c r="B78" s="5">
+        <v>2207</v>
+      </c>
+      <c r="C78" s="5" t="s">
         <v>91</v>
       </c>
-      <c r="D71" s="12"/>
-      <c r="G71" s="12"/>
-    </row>
-    <row r="72" ht="15.75" customHeight="1">
-      <c r="A72" s="9">
-        <v>184.0</v>
-      </c>
-      <c r="B72" s="9">
-        <v>862.0</v>
-      </c>
-      <c r="C72" s="9" t="s">
-        <v>92</v>
-      </c>
-      <c r="D72" s="12"/>
-      <c r="G72" s="12"/>
-    </row>
-    <row r="73" ht="15.75" customHeight="1">
-      <c r="A73" s="9">
-        <v>185.0</v>
-      </c>
-      <c r="B73" s="9">
-        <v>863.0</v>
-      </c>
-      <c r="C73" s="9" t="s">
-        <v>93</v>
-      </c>
-      <c r="D73" s="12"/>
-      <c r="G73" s="12"/>
-    </row>
-    <row r="74" ht="15.75" customHeight="1">
-      <c r="A74" s="9">
-        <v>186.0</v>
-      </c>
-      <c r="B74" s="9">
-        <v>864.0</v>
-      </c>
-      <c r="C74" s="9" t="s">
-        <v>94</v>
-      </c>
-      <c r="D74" s="12"/>
-      <c r="G74" s="12">
-        <v>2.000000184654E12</v>
-      </c>
-    </row>
-    <row r="75" ht="15.75" customHeight="1">
-      <c r="A75" s="9">
-        <v>187.0</v>
-      </c>
-      <c r="B75" s="9">
-        <v>865.0</v>
-      </c>
-      <c r="C75" s="9" t="s">
-        <v>95</v>
-      </c>
-      <c r="D75" s="12"/>
-      <c r="G75" s="12"/>
-    </row>
-    <row r="76" ht="15.75" customHeight="1">
-      <c r="A76" s="9">
-        <v>188.0</v>
-      </c>
-      <c r="B76" s="9">
-        <v>991.0</v>
-      </c>
-      <c r="C76" s="9" t="s">
-        <v>96</v>
-      </c>
-      <c r="I76" s="12">
-        <v>2.555477000001E12</v>
-      </c>
-    </row>
-    <row r="77" ht="15.75" customHeight="1">
-      <c r="A77" s="9">
-        <v>189.0</v>
-      </c>
-      <c r="B77" s="9">
-        <v>1082.0</v>
-      </c>
-      <c r="C77" s="9" t="s">
-        <v>97</v>
-      </c>
-    </row>
-    <row r="78" ht="15.75" customHeight="1">
-      <c r="A78" s="9">
-        <v>244.0</v>
-      </c>
-      <c r="B78" s="9">
-        <v>2207.0</v>
-      </c>
-      <c r="C78" s="9" t="s">
-        <v>98</v>
-      </c>
-    </row>
-    <row r="79" ht="15.75" customHeight="1"/>
-    <row r="80" ht="15.75" customHeight="1"/>
+    </row>
+    <row r="79" spans="1:9" ht="15.75" customHeight="1"/>
+    <row r="80" spans="1:9" ht="15.75" customHeight="1"/>
     <row r="81" ht="15.75" customHeight="1"/>
     <row r="82" ht="15.75" customHeight="1"/>
     <row r="83" ht="15.75" customHeight="1"/>
@@ -2787,24 +2669,20 @@
     <mergeCell ref="A1:C1"/>
     <mergeCell ref="D1:I1"/>
   </mergeCells>
-  <printOptions/>
-  <pageMargins bottom="0.75" footer="0.0" header="0.0" left="0.7" right="0.7" top="0.75"/>
-  <pageSetup orientation="portrait"/>
-  <drawing r:id="rId1"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0" footer="0"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:mv="urn:schemas-microsoft-com:mac:vml" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
-  <sheetPr>
-    <pageSetUpPr/>
-  </sheetPr>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
+  <dimension ref="A21:A1000"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr customHeight="1" defaultColWidth="14.43" defaultRowHeight="15.0"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="14.42578125" defaultRowHeight="15" customHeight="1"/>
   <cols>
-    <col customWidth="1" min="1" max="26" width="10.71"/>
+    <col min="1" max="26" width="10.7109375" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="21" ht="15.75" customHeight="1"/>
@@ -3788,24 +3666,20 @@
     <row r="999" ht="15.75" customHeight="1"/>
     <row r="1000" ht="15.75" customHeight="1"/>
   </sheetData>
-  <printOptions/>
-  <pageMargins bottom="0.75" footer="0.0" header="0.0" left="0.7" right="0.7" top="0.75"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0" footer="0"/>
   <pageSetup orientation="landscape"/>
-  <drawing r:id="rId1"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:mv="urn:schemas-microsoft-com:mac:vml" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
-  <sheetPr>
-    <pageSetUpPr/>
-  </sheetPr>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
+  <dimension ref="A21:A1000"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr customHeight="1" defaultColWidth="14.43" defaultRowHeight="15.0"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="14.42578125" defaultRowHeight="15" customHeight="1"/>
   <cols>
-    <col customWidth="1" min="1" max="26" width="10.71"/>
+    <col min="1" max="26" width="10.7109375" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="21" ht="15.75" customHeight="1"/>
@@ -4789,9 +4663,7 @@
     <row r="999" ht="15.75" customHeight="1"/>
     <row r="1000" ht="15.75" customHeight="1"/>
   </sheetData>
-  <printOptions/>
-  <pageMargins bottom="0.75" footer="0.0" header="0.0" left="0.7" right="0.7" top="0.75"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0" footer="0"/>
   <pageSetup orientation="landscape"/>
-  <drawing r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>